<commit_message>
Add análise final, plan
</commit_message>
<xml_diff>
--- a/Tabelas e Gráficos/Economia.xlsx
+++ b/Tabelas e Gráficos/Economia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhlui\OneDrive\Área de Trabalho\Luis Henrique\ESTUDOS\FIAP\Tech Challenge\Fase 3\bigdata_covid\Tabelas e Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F510144-699E-473C-A969-6AC36B85086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49575614-578E-452B-8FD7-582E9A64619F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35280" yWindow="0" windowWidth="10125" windowHeight="8340" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total por Mês" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="resul_escolaridade" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Escolaridade!$C$8:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Escolaridade!$C$8:$G$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">resul_escolaridade!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
   <si>
     <t>recebeu_auxilio</t>
   </si>
@@ -107,13 +107,19 @@
   </si>
   <si>
     <t>Pós-graduação</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>NÃO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +138,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,13 +182,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,16 +525,15 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>557240</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <f>VLOOKUP(A2,'Fez Exame'!A:D,4,0)</f>
         <v>56562</v>
       </c>
       <c r="D2">
-        <f>VLOOKUP(A2,'Resultados Exame'!A:C,2,0)</f>
-        <v>25761</v>
+        <v>30466</v>
       </c>
       <c r="E2">
         <f>Trabalho!C2</f>
@@ -530,7 +545,7 @@
       </c>
       <c r="H2" s="3">
         <f>D2/C2</f>
-        <v>0.45544711997454124</v>
+        <v>0.53863017573636007</v>
       </c>
       <c r="I2" s="3">
         <f>E2/B2</f>
@@ -541,16 +556,15 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>600744</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <f>VLOOKUP(A3,'Fez Exame'!A:D,4,0)</f>
         <v>37955</v>
       </c>
       <c r="D3">
-        <f>VLOOKUP(A3,'Resultados Exame'!A:C,2,0)</f>
-        <v>15248</v>
+        <v>22459</v>
       </c>
       <c r="E3">
         <f>Trabalho!C3</f>
@@ -562,11 +576,57 @@
       </c>
       <c r="H3" s="3">
         <f>D3/C3</f>
-        <v>0.40173890133052298</v>
+        <v>0.59172704518508756</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3" si="0">E3/B3</f>
         <v>0.31140718841969289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <f>B3/SUM($B$2:$B$3)</f>
+        <v>0.51878437007765221</v>
+      </c>
+      <c r="D5" s="3">
+        <f>D3/SUM($C$3)</f>
+        <v>0.59172704518508756</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <f>1-B5</f>
+        <v>0.48121562992234779</v>
+      </c>
+      <c r="D6" s="3">
+        <f>D2/SUM($C$2)</f>
+        <v>0.53863017573636007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>23673</v>
+      </c>
+      <c r="F11">
+        <v>129831</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>39132</v>
+      </c>
+      <c r="F12">
+        <v>140487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>E12/E11-1</f>
+        <v>0.65302243061715881</v>
+      </c>
+      <c r="F13" s="3">
+        <f>F12/F11-1</f>
+        <v>8.207592947755149E-2</v>
       </c>
     </row>
   </sheetData>
@@ -580,7 +640,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +745,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +785,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -732,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +903,15 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -851,9 +920,17 @@
       <c r="D9">
         <v>25907</v>
       </c>
-      <c r="E9" s="3">
-        <f>D9/$D$18</f>
+      <c r="E9">
+        <f>HLOOKUP(C9,$B$1:$I$3,3,0)</f>
+        <v>4202</v>
+      </c>
+      <c r="F9" s="3">
+        <f>D9/D$18</f>
         <v>4.6491637355538011E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f>E9/E$18</f>
+        <v>6.9946599549891471E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -863,9 +940,17 @@
       <c r="D10">
         <v>34708</v>
       </c>
-      <c r="E10" s="3">
-        <f t="shared" ref="E10:E16" si="0">D10/$D$18</f>
+      <c r="E10">
+        <f t="shared" ref="E10:E16" si="0">HLOOKUP(C10,$B$1:$I$3,3,0)</f>
+        <v>25471</v>
+      </c>
+      <c r="F10" s="3">
+        <f>D10/$D$18</f>
         <v>6.2285550211757947E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ref="G10:G16" si="1">E10/E$18</f>
+        <v>4.2399091792843541E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,9 +960,17 @@
       <c r="D11">
         <v>37055</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <f t="shared" si="0"/>
+        <v>39670</v>
+      </c>
+      <c r="F11" s="3">
+        <f>D11/$D$18</f>
         <v>6.6497379944009768E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="1"/>
+        <v>6.6034783535083158E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -887,9 +980,17 @@
       <c r="D12">
         <v>41817</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <f t="shared" si="0"/>
+        <v>66721</v>
+      </c>
+      <c r="F12" s="3">
+        <f>D12/$D$18</f>
         <v>7.5043069413538152E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11106394737192547</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -899,9 +1000,17 @@
       <c r="D13">
         <v>52433</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <f t="shared" si="0"/>
+        <v>72599</v>
+      </c>
+      <c r="F13" s="3">
+        <f>D13/$D$18</f>
         <v>9.4094106668580868E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12084848121662471</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -911,9 +1020,17 @@
       <c r="D14">
         <v>81272</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <f t="shared" si="0"/>
+        <v>27052</v>
+      </c>
+      <c r="F14" s="3">
+        <f>D14/$D$18</f>
         <v>0.14584739071136316</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="1"/>
+        <v>4.5030828439401809E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -923,9 +1040,17 @@
       <c r="D15">
         <v>121556</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <f t="shared" si="0"/>
+        <v>136336</v>
+      </c>
+      <c r="F15" s="3">
+        <f>D15/$D$18</f>
         <v>0.21813940133515183</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.22694525455102341</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,18 +1060,31 @@
       <c r="D16">
         <v>162492</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <f t="shared" si="0"/>
+        <v>228693</v>
+      </c>
+      <c r="F16" s="3">
+        <f>D16/$D$18</f>
         <v>0.29160146436006029</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
+        <f t="shared" si="1"/>
+        <v>0.38068295313810874</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18">
         <f>SUM(D9:D16)</f>
         <v>557240</v>
       </c>
+      <c r="E18">
+        <f>SUM(E9:E16)</f>
+        <v>600744</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="C8:G16" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="B2:I2">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -1235,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>